<commit_message>
feat(admin): add giveAuthority endpoint and role management
- introduced giveAuthority function in adminController.js to assign user roles (e.g., moderator)
- added levelMap and powerMap to adminController.js and removed duplicate from userController.js
- updated admin.js routes to include /giveAuthority/:userID with proper authorization middleware
- extended permissions in authVerification.js to include GIVE_AUTHORITY_MODERATOR
</commit_message>
<xml_diff>
--- a/docs/status_codes.xlsx
+++ b/docs/status_codes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>001</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>You cannot restrict someone with a high or same rank</t>
+  </si>
+  <si>
+    <t>successfully unrestricted</t>
+  </si>
+  <si>
+    <t>Granted authority</t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,7 @@
   <dimension ref="F5:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,10 +938,16 @@
       <c r="F46" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="G46" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F47" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="G47" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>